<commit_message>
update xls tables for cmcc-esm2
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
+++ b/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-cm2-sr5/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFED641-766F-8243-8A5D-029F421B0794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="460">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -37,7 +43,7 @@
     <t>Model</t>
   </si>
   <si>
-    <t>CMCC-ESM2</t>
+    <t>CMCC-CM2-SR5</t>
   </si>
   <si>
     <t>Realm / Topic</t>
@@ -1277,13 +1283,133 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>RRTMg</t>
+  </si>
+  <si>
+    <t>low top: concentrations from high top simulations; high top: from precursors, using full chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> emission precursors</t>
+  </si>
+  <si>
+    <t>emission precursors; secondary organic aerosols in high-top use VBS scheme</t>
+  </si>
+  <si>
+    <t>Prognostic</t>
+  </si>
+  <si>
+    <t>Emission</t>
+  </si>
+  <si>
+    <t>SO2 emissions</t>
+  </si>
+  <si>
+    <t>SO2 emissions in high-top; concentration in low-top, from high-top simulations</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Explicit modeling of the radiative effects of land use change using the Land Use Harmonization version 2 (LUH2) dataset.</t>
+  </si>
+  <si>
+    <t>Land Use Harmonization version 2 (LUH2) is used after conversion to CLM plant functional and landunit types.</t>
+  </si>
+  <si>
+    <t>CMCC, CESM, climate model</t>
+  </si>
+  <si>
+    <t>No fluxes corrections are used in the model.</t>
+  </si>
+  <si>
+    <t>CMCC-CESM</t>
+  </si>
+  <si>
+    <t>Fortran, C, Python, Perl</t>
+  </si>
+  <si>
+    <t>The top-level, independent components are: atmosphere (CAM), land (CLM), ocean (NEMO), sea ice (CICE), river (RTM). These components are coupled to each other via a hub-and-spoke coupling architecture (CPL).</t>
+  </si>
+  <si>
+    <t>CPL6/MCT</t>
+  </si>
+  <si>
+    <t>In comparison to its previous version, the model contains many substantial science and infrastructure changes and improvements in all its components. These new advancements include: a different atmospheric model component (CAM) that incorporates significantly advanced features for turbulence and convection representations; a different land model component (CLM) with increase number of PFT components and updated land processes representation; a community based seaice model (CICE) with state of the art thermodyanics formulations and additioanl parameerizations; an updated ocean component (NEMO) with additional features to describe ocean interior dynamics, small scale paramterizations and improved computational capabilities.</t>
+  </si>
+  <si>
+    <t>The details of the model tuning will be described in the CMCC model description manuscript. The primary tuning involved the top-of-the-atmosphere (TOA) heat flux in pre-industrial control simulations. Our desire was to achive a rather small TOA (e.g. &lt; 0.1 W m^-2), mostly working on atmospheric aerosol indiret effects and land processes related to the snow cycle in northern emisphere.</t>
+  </si>
+  <si>
+    <t>top-of-the-atmosphere (TOA) heat flux, global-mean ocean temperature, sea-ice extent, sea-ice volume, glacial mass balance, etc.</t>
+  </si>
+  <si>
+    <t>Ocean meridional overturning circulation,  sea-ice distributions, snow cover on nothern emisphere</t>
+  </si>
+  <si>
+    <t>Adjustments of aerosol indirect effect</t>
+  </si>
+  <si>
+    <t>Both the coupled system and the individual model components conserve heat.</t>
+  </si>
+  <si>
+    <t>Both the coupled system and the individual model components conserve freshwater / salt (at best of used formulations)</t>
+  </si>
+  <si>
+    <t>In the coupled configurations, surface heat fluxes are exchanged across the component models in a fully conservative way.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All flux exchanges are done in a fully conservative way. </t>
+  </si>
+  <si>
+    <t>Heat is conserved through the coupler except that the heat content of precipitating water is not tracked.</t>
+  </si>
+  <si>
+    <t>Stream temperature is not modeled thus there is no heat exchange between the land and the ocean.</t>
+  </si>
+  <si>
+    <t>All freshwater and salt flux exchanges are fully conserved.</t>
+  </si>
+  <si>
+    <t>All freshwater flux exchanges are fully conserved.</t>
+  </si>
+  <si>
+    <t>Fresh water is conserved through the coupler.</t>
+  </si>
+  <si>
+    <t>A river routing scheme is used. All liquid and frozen runoff fluxes are sent to the ocean model using conservative mappings.</t>
+  </si>
+  <si>
+    <t>The salt / freshwater content of these basins are kept constant throughout a simulation using a marginal sea balancing scheme where access (deficit) freshwater is sent to (taken from) the nearest ocean point.</t>
+  </si>
+  <si>
+    <t>All salt exchanges between the ocean and sea ice models are done conservatively.</t>
+  </si>
+  <si>
+    <t>Tomas Lovato</t>
+  </si>
+  <si>
+    <t>LOVATO-TOMAS</t>
+  </si>
+  <si>
+    <t>Point of Contact</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>GUALDI-SILVIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1479,6 +1605,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1525,7 +1659,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1557,9 +1691,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1591,6 +1743,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1766,24 +1936,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1791,7 +1963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1807,7 +1979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1823,12 +1995,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +2008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1844,7 +2016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1852,7 +2024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1860,13 +2032,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1874,54 +2048,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1929,70 +2105,84 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="9" t="s">
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B10" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Radiative Forcings"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD224"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -2000,12 +2190,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -2013,7 +2203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -2024,10 +2214,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -2035,7 +2227,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>37</v>
       </c>
@@ -2046,15 +2238,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -2062,7 +2256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>37</v>
       </c>
@@ -2073,15 +2267,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
+    <row r="16" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>50</v>
       </c>
@@ -2089,12 +2283,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
+    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>53</v>
       </c>
@@ -2102,7 +2296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -2113,15 +2307,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="28" spans="1:3" ht="24" customHeight="1">
+    <row r="25" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
@@ -2129,12 +2325,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1">
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>60</v>
       </c>
@@ -2142,7 +2338,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="24" customHeight="1">
+    <row r="32" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>37</v>
       </c>
@@ -2153,10 +2349,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
-    </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>64</v>
       </c>
@@ -2164,7 +2362,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
+    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>37</v>
       </c>
@@ -2175,10 +2373,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>68</v>
       </c>
@@ -2186,7 +2384,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
+    <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>37</v>
       </c>
@@ -2197,10 +2395,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
-    </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>72</v>
       </c>
@@ -2208,7 +2408,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
+    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>37</v>
       </c>
@@ -2219,15 +2419,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
+    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
-      <c r="B46" s="11"/>
-    </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
+    <row r="46" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>76</v>
       </c>
@@ -2235,7 +2437,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="24" customHeight="1">
+    <row r="49" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>37</v>
       </c>
@@ -2246,10 +2448,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24" customHeight="1">
+    <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="11"/>
     </row>
-    <row r="53" spans="1:3" ht="24" customHeight="1">
+    <row r="53" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>80</v>
       </c>
@@ -2257,12 +2459,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="24" customHeight="1">
+    <row r="54" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="24" customHeight="1">
+    <row r="56" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>83</v>
       </c>
@@ -2270,7 +2472,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="24" customHeight="1">
+    <row r="57" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
@@ -2281,10 +2483,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="24" customHeight="1">
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="11"/>
     </row>
-    <row r="60" spans="1:3" ht="24" customHeight="1">
+    <row r="60" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>87</v>
       </c>
@@ -2292,7 +2494,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="24" customHeight="1">
+    <row r="61" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>37</v>
       </c>
@@ -2303,10 +2505,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="24" customHeight="1">
+    <row r="62" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="11"/>
     </row>
-    <row r="64" spans="1:3" ht="24" customHeight="1">
+    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>91</v>
       </c>
@@ -2314,7 +2516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="24" customHeight="1">
+    <row r="65" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>37</v>
       </c>
@@ -2325,15 +2527,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="24" customHeight="1">
+    <row r="66" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
-    </row>
-    <row r="69" spans="1:34" ht="24" customHeight="1">
+    <row r="67" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>95</v>
       </c>
@@ -2341,7 +2545,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="24" customHeight="1">
+    <row r="70" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
         <v>37</v>
       </c>
@@ -2352,10 +2556,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
-    </row>
-    <row r="73" spans="1:34" ht="24" customHeight="1">
+    <row r="71" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="73" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>99</v>
       </c>
@@ -2363,7 +2569,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="24" customHeight="1">
+    <row r="74" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>101</v>
       </c>
@@ -2374,8 +2580,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+    <row r="75" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>437</v>
+      </c>
       <c r="AA75" s="6" t="s">
         <v>104</v>
       </c>
@@ -2401,7 +2612,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="24" customHeight="1">
+    <row r="78" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>112</v>
       </c>
@@ -2409,10 +2620,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="24" customHeight="1">
+    <row r="79" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="13"/>
     </row>
-    <row r="81" spans="1:30" ht="24" customHeight="1">
+    <row r="81" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>114</v>
       </c>
@@ -2420,7 +2631,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="24" customHeight="1">
+    <row r="82" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>116</v>
       </c>
@@ -2431,10 +2642,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="24" customHeight="1">
-      <c r="B83" s="11"/>
-    </row>
-    <row r="85" spans="1:30" ht="24" customHeight="1">
+    <row r="83" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>119</v>
       </c>
@@ -2442,7 +2655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="24" customHeight="1">
+    <row r="86" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
         <v>101</v>
       </c>
@@ -2453,8 +2666,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+    <row r="87" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="AA87" s="6" t="s">
         <v>123</v>
       </c>
@@ -2468,7 +2683,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="24" customHeight="1">
+    <row r="89" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2476,7 +2691,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="24" customHeight="1">
+    <row r="90" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
         <v>116</v>
       </c>
@@ -2487,10 +2702,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
-    </row>
-    <row r="94" spans="1:30" ht="24" customHeight="1">
+    <row r="91" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
         <v>130</v>
       </c>
@@ -2498,12 +2715,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="24" customHeight="1">
+    <row r="95" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24" customHeight="1">
+    <row r="97" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2511,7 +2728,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="24" customHeight="1">
+    <row r="98" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
         <v>37</v>
       </c>
@@ -2522,15 +2739,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="24" customHeight="1">
+    <row r="99" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="178" customHeight="1">
-      <c r="B100" s="11"/>
-    </row>
-    <row r="102" spans="1:3" ht="24" customHeight="1">
+    <row r="100" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>137</v>
       </c>
@@ -2538,7 +2757,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
+    <row r="103" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
         <v>37</v>
       </c>
@@ -2549,15 +2768,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
+    <row r="104" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
-    </row>
-    <row r="107" spans="1:3" ht="24" customHeight="1">
+    <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>141</v>
       </c>
@@ -2565,7 +2786,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="24" customHeight="1">
+    <row r="108" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
         <v>37</v>
       </c>
@@ -2576,15 +2797,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="24" customHeight="1">
+    <row r="109" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="24" customHeight="1">
-      <c r="B110" s="11"/>
-    </row>
-    <row r="112" spans="1:3" ht="24" customHeight="1">
+    <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>145</v>
       </c>
@@ -2592,7 +2815,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24" customHeight="1">
+    <row r="113" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
         <v>37</v>
       </c>
@@ -2603,15 +2826,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="24" customHeight="1">
+    <row r="114" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="24" customHeight="1">
-      <c r="B115" s="11"/>
-    </row>
-    <row r="117" spans="1:3" ht="24" customHeight="1">
+    <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
         <v>149</v>
       </c>
@@ -2619,7 +2844,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="24" customHeight="1">
+    <row r="118" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
         <v>37</v>
       </c>
@@ -2630,10 +2855,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="24" customHeight="1">
-      <c r="B119" s="11"/>
-    </row>
-    <row r="121" spans="1:3" ht="24" customHeight="1">
+    <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B119" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
         <v>153</v>
       </c>
@@ -2641,7 +2868,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="24" customHeight="1">
+    <row r="122" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
         <v>37</v>
       </c>
@@ -2652,10 +2879,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="24" customHeight="1">
-      <c r="B123" s="11"/>
-    </row>
-    <row r="126" spans="1:3" ht="24" customHeight="1">
+    <row r="123" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
         <v>157</v>
       </c>
@@ -2663,12 +2892,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24" customHeight="1">
+    <row r="127" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" customHeight="1">
+    <row r="129" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
         <v>160</v>
       </c>
@@ -2676,7 +2905,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="24" customHeight="1">
+    <row r="130" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
         <v>37</v>
       </c>
@@ -2687,15 +2916,17 @@
         <v>163</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="24" customHeight="1">
+    <row r="131" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="178" customHeight="1">
-      <c r="B132" s="11"/>
-    </row>
-    <row r="134" spans="1:3" ht="24" customHeight="1">
+    <row r="132" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
         <v>164</v>
       </c>
@@ -2703,7 +2934,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="24" customHeight="1">
+    <row r="135" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
         <v>37</v>
       </c>
@@ -2714,15 +2945,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="24" customHeight="1">
+    <row r="136" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="178" customHeight="1">
-      <c r="B137" s="11"/>
-    </row>
-    <row r="139" spans="1:3" ht="24" customHeight="1">
+    <row r="137" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
         <v>168</v>
       </c>
@@ -2730,7 +2963,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" customHeight="1">
+    <row r="140" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="14" t="s">
         <v>37</v>
       </c>
@@ -2741,15 +2974,17 @@
         <v>171</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="24" customHeight="1">
+    <row r="141" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="178" customHeight="1">
-      <c r="B142" s="11"/>
-    </row>
-    <row r="144" spans="1:3" ht="24" customHeight="1">
+    <row r="142" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>172</v>
       </c>
@@ -2757,7 +2992,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="24" customHeight="1">
+    <row r="145" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="14" t="s">
         <v>37</v>
       </c>
@@ -2768,15 +3003,17 @@
         <v>175</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="24" customHeight="1">
+    <row r="146" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="178" customHeight="1">
-      <c r="B147" s="11"/>
-    </row>
-    <row r="149" spans="1:3" ht="24" customHeight="1">
+    <row r="147" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B147" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>176</v>
       </c>
@@ -2784,7 +3021,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="24" customHeight="1">
+    <row r="150" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="14" t="s">
         <v>37</v>
       </c>
@@ -2795,15 +3032,17 @@
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="24" customHeight="1">
+    <row r="151" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="178" customHeight="1">
-      <c r="B152" s="11"/>
-    </row>
-    <row r="154" spans="1:3" ht="24" customHeight="1">
+    <row r="152" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B152" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="9" t="s">
         <v>180</v>
       </c>
@@ -2811,7 +3050,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="24" customHeight="1">
+    <row r="155" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="14" t="s">
         <v>37</v>
       </c>
@@ -2822,15 +3061,17 @@
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="24" customHeight="1">
+    <row r="156" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="178" customHeight="1">
-      <c r="B157" s="11"/>
-    </row>
-    <row r="160" spans="1:3" ht="24" customHeight="1">
+    <row r="157" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B157" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
         <v>184</v>
       </c>
@@ -2838,12 +3079,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="24" customHeight="1">
+    <row r="161" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="24" customHeight="1">
+    <row r="163" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
         <v>187</v>
       </c>
@@ -2851,7 +3092,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="24" customHeight="1">
+    <row r="164" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="14" t="s">
         <v>37</v>
       </c>
@@ -2862,15 +3103,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="24" customHeight="1">
+    <row r="165" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="178" customHeight="1">
-      <c r="B166" s="11"/>
-    </row>
-    <row r="168" spans="1:3" ht="24" customHeight="1">
+    <row r="166" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>190</v>
       </c>
@@ -2878,7 +3121,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="24" customHeight="1">
+    <row r="169" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="14" t="s">
         <v>37</v>
       </c>
@@ -2889,15 +3132,17 @@
         <v>192</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="24" customHeight="1">
+    <row r="170" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="178" customHeight="1">
-      <c r="B171" s="11"/>
-    </row>
-    <row r="173" spans="1:3" ht="24" customHeight="1">
+    <row r="171" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B171" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
         <v>193</v>
       </c>
@@ -2905,7 +3150,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="24" customHeight="1">
+    <row r="174" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="14" t="s">
         <v>37</v>
       </c>
@@ -2916,15 +3161,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="24" customHeight="1">
+    <row r="175" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="178" customHeight="1">
-      <c r="B176" s="11"/>
-    </row>
-    <row r="178" spans="1:3" ht="24" customHeight="1">
+    <row r="176" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B176" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="9" t="s">
         <v>196</v>
       </c>
@@ -2932,7 +3179,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="24" customHeight="1">
+    <row r="179" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="14" t="s">
         <v>37</v>
       </c>
@@ -2943,15 +3190,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="24" customHeight="1">
+    <row r="180" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="178" customHeight="1">
-      <c r="B181" s="11"/>
-    </row>
-    <row r="183" spans="1:3" ht="24" customHeight="1">
+    <row r="181" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B181" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="9" t="s">
         <v>199</v>
       </c>
@@ -2959,7 +3208,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="24" customHeight="1">
+    <row r="184" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="14" t="s">
         <v>37</v>
       </c>
@@ -2970,15 +3219,17 @@
         <v>201</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="24" customHeight="1">
+    <row r="185" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="178" customHeight="1">
-      <c r="B186" s="11"/>
-    </row>
-    <row r="188" spans="1:3" ht="24" customHeight="1">
+    <row r="186" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B186" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="9" t="s">
         <v>202</v>
       </c>
@@ -2986,7 +3237,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="24" customHeight="1">
+    <row r="189" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="14" t="s">
         <v>37</v>
       </c>
@@ -2997,15 +3248,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="24" customHeight="1">
+    <row r="190" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="178" customHeight="1">
-      <c r="B191" s="11"/>
-    </row>
-    <row r="193" spans="1:3" ht="24" customHeight="1">
+    <row r="191" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B191" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="9" t="s">
         <v>206</v>
       </c>
@@ -3013,7 +3266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="24" customHeight="1">
+    <row r="194" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="14" t="s">
         <v>37</v>
       </c>
@@ -3024,15 +3277,15 @@
         <v>209</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="24" customHeight="1">
+    <row r="195" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="178" customHeight="1">
+    <row r="196" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="11"/>
     </row>
-    <row r="198" spans="1:3" ht="24" customHeight="1">
+    <row r="198" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="9" t="s">
         <v>210</v>
       </c>
@@ -3040,7 +3293,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="24" customHeight="1">
+    <row r="199" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="14" t="s">
         <v>37</v>
       </c>
@@ -3051,15 +3304,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="24" customHeight="1">
+    <row r="200" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="178" customHeight="1">
-      <c r="B201" s="11"/>
-    </row>
-    <row r="203" spans="1:3" ht="24" customHeight="1">
+    <row r="201" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B201" s="11" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="9" t="s">
         <v>214</v>
       </c>
@@ -3067,7 +3322,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="24" customHeight="1">
+    <row r="204" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="14" t="s">
         <v>37</v>
       </c>
@@ -3078,15 +3333,15 @@
         <v>217</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="24" customHeight="1">
+    <row r="205" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="178" customHeight="1">
+    <row r="206" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="11"/>
     </row>
-    <row r="209" spans="1:3" ht="24" customHeight="1">
+    <row r="209" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="12" t="s">
         <v>218</v>
       </c>
@@ -3094,12 +3349,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="24" customHeight="1">
+    <row r="210" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="24" customHeight="1">
+    <row r="212" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="9" t="s">
         <v>221</v>
       </c>
@@ -3107,7 +3362,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="24" customHeight="1">
+    <row r="213" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="14" t="s">
         <v>37</v>
       </c>
@@ -3118,15 +3373,17 @@
         <v>223</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="24" customHeight="1">
+    <row r="214" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="178" customHeight="1">
-      <c r="B215" s="11"/>
-    </row>
-    <row r="218" spans="1:3" ht="24" customHeight="1">
+    <row r="215" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B215" s="11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="12" t="s">
         <v>224</v>
       </c>
@@ -3134,12 +3391,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="24" customHeight="1">
+    <row r="219" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="13" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="24" customHeight="1">
+    <row r="221" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="9" t="s">
         <v>227</v>
       </c>
@@ -3147,7 +3404,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="24" customHeight="1">
+    <row r="222" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="14" t="s">
         <v>37</v>
       </c>
@@ -3158,27 +3415,24 @@
         <v>229</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="24" customHeight="1">
+    <row r="223" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="178" customHeight="1">
+    <row r="224" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA75:AH75</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83 B91" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>AA87:AD87</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3186,20 +3440,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AG300"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>230</v>
       </c>
@@ -3207,12 +3463,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>233</v>
       </c>
@@ -3220,7 +3476,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -3231,10 +3487,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>236</v>
       </c>
@@ -3242,7 +3500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>37</v>
       </c>
@@ -3253,15 +3511,15 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>239</v>
       </c>
@@ -3269,12 +3527,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="24" customHeight="1">
+    <row r="17" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>242</v>
       </c>
@@ -3282,7 +3540,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="24" customHeight="1">
+    <row r="18" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>101</v>
       </c>
@@ -3293,13 +3551,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="24" customHeight="1">
+    <row r="19" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>248</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>246</v>
       </c>
@@ -3322,1893 +3582,1945 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="24" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="21" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA21" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB21" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC21" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE21" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF21" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B23" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="24" customHeight="1">
-      <c r="A23" s="14" t="s">
+    <row r="24" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="24" customHeight="1">
-      <c r="B24" s="8" t="s">
+    <row r="25" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="28" spans="1:33" ht="24" customHeight="1">
-      <c r="A28" s="12" t="s">
+    <row r="26" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+    </row>
+    <row r="29" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="12" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="24" customHeight="1">
-      <c r="B29" s="13" t="s">
+    <row r="30" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="13" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="24" customHeight="1">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="24" customHeight="1">
-      <c r="A32" s="14" t="s">
+    <row r="33" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B33" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="24" customHeight="1">
-      <c r="B33" s="10" t="s">
+    <row r="34" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="24" customHeight="1">
-      <c r="B34" s="11"/>
-      <c r="AA34" s="6" t="s">
+    <row r="35" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA35" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB34" s="6" t="s">
+      <c r="AB35" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC34" s="6" t="s">
+      <c r="AC35" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD34" s="6" t="s">
+      <c r="AD35" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE34" s="6" t="s">
+      <c r="AE35" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF34" s="6" t="s">
+      <c r="AF35" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG34" s="6" t="s">
+      <c r="AG35" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="24" customHeight="1">
-      <c r="A36" s="9" t="s">
+    <row r="37" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="24" customHeight="1">
-      <c r="A37" s="14" t="s">
+    <row r="38" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="24" customHeight="1">
-      <c r="B38" s="8" t="s">
+    <row r="39" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="178" customHeight="1">
-      <c r="B39" s="11"/>
-    </row>
-    <row r="42" spans="1:33" ht="24" customHeight="1">
-      <c r="A42" s="12" t="s">
+    <row r="40" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="11"/>
+    </row>
+    <row r="43" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B43" s="12" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="24" customHeight="1">
-      <c r="B43" s="13" t="s">
+    <row r="44" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="13" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="24" customHeight="1">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B46" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="24" customHeight="1">
-      <c r="A46" s="14" t="s">
+    <row r="47" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B47" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="24" customHeight="1">
-      <c r="B47" s="10" t="s">
+    <row r="48" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="24" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="AA48" s="6" t="s">
+    <row r="49" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA49" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB48" s="6" t="s">
+      <c r="AB49" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC48" s="6" t="s">
+      <c r="AC49" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD48" s="6" t="s">
+      <c r="AD49" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE48" s="6" t="s">
+      <c r="AE49" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF48" s="6" t="s">
+      <c r="AF49" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG48" s="6" t="s">
+      <c r="AG49" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="24" customHeight="1">
-      <c r="A50" s="9" t="s">
+    <row r="51" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="24" customHeight="1">
-      <c r="A51" s="14" t="s">
+    <row r="52" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C52" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="24" customHeight="1">
-      <c r="B52" s="8" t="s">
+    <row r="53" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="178" customHeight="1">
-      <c r="B53" s="11"/>
-    </row>
-    <row r="56" spans="1:33" ht="24" customHeight="1">
-      <c r="A56" s="12" t="s">
+    <row r="54" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="11"/>
+    </row>
+    <row r="57" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B57" s="12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="24" customHeight="1">
-      <c r="B57" s="13" t="s">
+    <row r="58" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="13" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="24" customHeight="1">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B60" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="24" customHeight="1">
-      <c r="A60" s="14" t="s">
+    <row r="61" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B61" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="24" customHeight="1">
-      <c r="B61" s="10" t="s">
+    <row r="62" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
-      <c r="AA62" s="6" t="s">
+    <row r="63" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="11"/>
+      <c r="AA63" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB62" s="6" t="s">
+      <c r="AB63" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC62" s="6" t="s">
+      <c r="AC63" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD62" s="6" t="s">
+      <c r="AD63" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE62" s="6" t="s">
+      <c r="AE63" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF62" s="6" t="s">
+      <c r="AF63" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG62" s="6" t="s">
+      <c r="AG63" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="24" customHeight="1">
-      <c r="A64" s="9" t="s">
+    <row r="65" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="24" customHeight="1">
-      <c r="A65" s="14" t="s">
+    <row r="66" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B66" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C66" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="24" customHeight="1">
-      <c r="B66" s="8" t="s">
+    <row r="67" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="178" customHeight="1">
-      <c r="B67" s="11"/>
-    </row>
-    <row r="70" spans="1:33" ht="24" customHeight="1">
-      <c r="A70" s="12" t="s">
+    <row r="68" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="11"/>
+    </row>
+    <row r="71" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B71" s="12" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="24" customHeight="1">
-      <c r="B71" s="13" t="s">
+    <row r="72" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="13" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="24" customHeight="1">
-      <c r="A73" s="9" t="s">
+    <row r="74" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="24" customHeight="1">
-      <c r="A74" s="14" t="s">
+    <row r="75" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B75" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C75" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="24" customHeight="1">
-      <c r="B75" s="10" t="s">
+    <row r="76" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="24" customHeight="1">
-      <c r="B76" s="11"/>
-      <c r="AA76" s="6" t="s">
+    <row r="77" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="AA77" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB76" s="6" t="s">
+      <c r="AB77" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC76" s="6" t="s">
+      <c r="AC77" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD76" s="6" t="s">
+      <c r="AD77" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE76" s="6" t="s">
+      <c r="AE77" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF76" s="6" t="s">
+      <c r="AF77" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG76" s="6" t="s">
+      <c r="AG77" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="24" customHeight="1">
-      <c r="A78" s="9" t="s">
+    <row r="79" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="24" customHeight="1">
-      <c r="A79" s="14" t="s">
+    <row r="80" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B80" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C80" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="24" customHeight="1">
-      <c r="B80" s="8" t="s">
+    <row r="81" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="178" customHeight="1">
-      <c r="B81" s="11"/>
-    </row>
-    <row r="84" spans="1:33" ht="24" customHeight="1">
-      <c r="A84" s="12" t="s">
+    <row r="82" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="11"/>
+    </row>
+    <row r="85" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B85" s="12" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="24" customHeight="1">
-      <c r="B85" s="13" t="s">
+    <row r="86" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="13" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="24" customHeight="1">
-      <c r="A87" s="9" t="s">
+    <row r="88" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B88" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="24" customHeight="1">
-      <c r="A88" s="14" t="s">
+    <row r="89" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B89" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C89" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="24" customHeight="1">
-      <c r="B89" s="10" t="s">
+    <row r="90" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="24" customHeight="1">
-      <c r="B90" s="11"/>
-      <c r="AA90" s="6" t="s">
+    <row r="91" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA91" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB90" s="6" t="s">
+      <c r="AB91" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC90" s="6" t="s">
+      <c r="AC91" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD90" s="6" t="s">
+      <c r="AD91" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE90" s="6" t="s">
+      <c r="AE91" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF90" s="6" t="s">
+      <c r="AF91" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG90" s="6" t="s">
+      <c r="AG91" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="24" customHeight="1">
-      <c r="A92" s="9" t="s">
+    <row r="93" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B93" s="9" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="24" customHeight="1">
-      <c r="A93" s="14" t="s">
+    <row r="94" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B94" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C94" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="24" customHeight="1">
-      <c r="B94" s="11"/>
-      <c r="AA94" s="6" t="s">
+    <row r="95" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="11"/>
+      <c r="AA95" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="AB94" s="6" t="s">
+      <c r="AB95" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="AC94" s="6" t="s">
+      <c r="AC95" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="AD94" s="6" t="s">
+      <c r="AD95" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="AE94" s="6" t="s">
+      <c r="AE95" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="24" customHeight="1">
-      <c r="A96" s="9" t="s">
+    <row r="97" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B97" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="97" spans="1:33" ht="24" customHeight="1">
-      <c r="A97" s="14" t="s">
+    <row r="98" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B98" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C98" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="98" spans="1:33" ht="24" customHeight="1">
-      <c r="B98" s="8" t="s">
+    <row r="99" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="178" customHeight="1">
-      <c r="B99" s="11"/>
-    </row>
-    <row r="102" spans="1:33" ht="24" customHeight="1">
-      <c r="A102" s="12" t="s">
+    <row r="100" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="11"/>
+    </row>
+    <row r="103" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B103" s="12" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:33" ht="24" customHeight="1">
-      <c r="B103" s="13" t="s">
+    <row r="104" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="13" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="105" spans="1:33" ht="24" customHeight="1">
-      <c r="A105" s="9" t="s">
+    <row r="106" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B106" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="1:33" ht="24" customHeight="1">
-      <c r="A106" s="14" t="s">
+    <row r="107" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B107" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C107" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="107" spans="1:33" ht="24" customHeight="1">
-      <c r="B107" s="10" t="s">
+    <row r="108" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:33" ht="24" customHeight="1">
-      <c r="B108" s="11"/>
-      <c r="AA108" s="6" t="s">
+    <row r="109" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="AA109" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB108" s="6" t="s">
+      <c r="AB109" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC108" s="6" t="s">
+      <c r="AC109" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD108" s="6" t="s">
+      <c r="AD109" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE108" s="6" t="s">
+      <c r="AE109" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF108" s="6" t="s">
+      <c r="AF109" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG108" s="6" t="s">
+      <c r="AG109" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:33" ht="24" customHeight="1">
-      <c r="A110" s="9" t="s">
+    <row r="111" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:33" ht="24" customHeight="1">
-      <c r="A111" s="14" t="s">
+    <row r="112" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B112" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C111" s="10" t="s">
+      <c r="C112" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="112" spans="1:33" ht="24" customHeight="1">
-      <c r="B112" s="8" t="s">
+    <row r="113" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="113" spans="1:33" ht="178" customHeight="1">
-      <c r="B113" s="11"/>
-    </row>
-    <row r="116" spans="1:33" ht="24" customHeight="1">
-      <c r="A116" s="12" t="s">
+    <row r="114" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="11"/>
+    </row>
+    <row r="117" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B117" s="12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="117" spans="1:33" ht="24" customHeight="1">
-      <c r="B117" s="13" t="s">
+    <row r="118" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="119" spans="1:33" ht="24" customHeight="1">
-      <c r="A119" s="9" t="s">
+    <row r="120" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B120" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="120" spans="1:33" ht="24" customHeight="1">
-      <c r="A120" s="14" t="s">
+    <row r="121" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B121" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C121" s="10" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="121" spans="1:33" ht="24" customHeight="1">
-      <c r="B121" s="10" t="s">
+    <row r="122" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:33" ht="24" customHeight="1">
-      <c r="B122" s="11"/>
-      <c r="AA122" s="6" t="s">
+    <row r="123" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="AA123" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB122" s="6" t="s">
+      <c r="AB123" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC122" s="6" t="s">
+      <c r="AC123" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD122" s="6" t="s">
+      <c r="AD123" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE122" s="6" t="s">
+      <c r="AE123" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF122" s="6" t="s">
+      <c r="AF123" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG122" s="6" t="s">
+      <c r="AG123" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:33" ht="24" customHeight="1">
-      <c r="A124" s="9" t="s">
+    <row r="125" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B125" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="125" spans="1:33" ht="24" customHeight="1">
-      <c r="A125" s="14" t="s">
+    <row r="126" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="B126" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C125" s="10" t="s">
+      <c r="C126" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="126" spans="1:33" ht="24" customHeight="1">
-      <c r="B126" s="8" t="s">
+    <row r="127" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="178" customHeight="1">
-      <c r="B127" s="11"/>
-    </row>
-    <row r="130" spans="1:33" ht="24" customHeight="1">
-      <c r="A130" s="12" t="s">
+    <row r="128" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="11"/>
+    </row>
+    <row r="131" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B131" s="12" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="131" spans="1:33" ht="24" customHeight="1">
-      <c r="B131" s="13" t="s">
+    <row r="132" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="13" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="133" spans="1:33" ht="24" customHeight="1">
-      <c r="A133" s="9" t="s">
+    <row r="134" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B134" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="134" spans="1:33" ht="24" customHeight="1">
-      <c r="A134" s="14" t="s">
+    <row r="135" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B134" s="10" t="s">
+      <c r="B135" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C134" s="10" t="s">
+      <c r="C135" s="10" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="135" spans="1:33" ht="24" customHeight="1">
-      <c r="B135" s="10" t="s">
+    <row r="136" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:33" ht="24" customHeight="1">
-      <c r="B136" s="11"/>
-      <c r="AA136" s="6" t="s">
+    <row r="137" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="AA137" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB136" s="6" t="s">
+      <c r="AB137" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC136" s="6" t="s">
+      <c r="AC137" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD136" s="6" t="s">
+      <c r="AD137" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE136" s="6" t="s">
+      <c r="AE137" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF136" s="6" t="s">
+      <c r="AF137" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG136" s="6" t="s">
+      <c r="AG137" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="138" spans="1:33" ht="24" customHeight="1">
-      <c r="A138" s="9" t="s">
+    <row r="139" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="B138" s="9" t="s">
+      <c r="B139" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="1:33" ht="24" customHeight="1">
-      <c r="A139" s="14" t="s">
+    <row r="140" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="B140" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C139" s="10" t="s">
+      <c r="C140" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="140" spans="1:33" ht="24" customHeight="1">
-      <c r="B140" s="8" t="s">
+    <row r="141" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B141" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:33" ht="178" customHeight="1">
-      <c r="B141" s="11"/>
-    </row>
-    <row r="144" spans="1:33" ht="24" customHeight="1">
-      <c r="A144" s="12" t="s">
+    <row r="142" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="11"/>
+    </row>
+    <row r="145" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B145" s="12" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="145" spans="1:33" ht="24" customHeight="1">
-      <c r="B145" s="13" t="s">
+    <row r="146" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B146" s="13" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="147" spans="1:33" ht="24" customHeight="1">
-      <c r="A147" s="9" t="s">
+    <row r="148" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B148" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="148" spans="1:33" ht="24" customHeight="1">
-      <c r="A148" s="14" t="s">
+    <row r="149" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B149" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C148" s="10" t="s">
+      <c r="C149" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="149" spans="1:33" ht="24" customHeight="1">
-      <c r="B149" s="10" t="s">
+    <row r="150" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B150" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:33" ht="24" customHeight="1">
-      <c r="B150" s="11"/>
-      <c r="AA150" s="6" t="s">
+    <row r="151" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B151" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="AB150" s="6" t="s">
+      <c r="AA151" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB151" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC150" s="6" t="s">
+      <c r="AC151" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD150" s="6" t="s">
+      <c r="AD151" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE150" s="6" t="s">
+      <c r="AE151" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF150" s="6" t="s">
+      <c r="AF151" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG150" s="6" t="s">
+      <c r="AG151" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="152" spans="1:33" ht="24" customHeight="1">
-      <c r="A152" s="9" t="s">
+    <row r="153" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B153" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="153" spans="1:33" ht="24" customHeight="1">
-      <c r="A153" s="14" t="s">
+    <row r="154" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B153" s="10" t="s">
+      <c r="B154" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C154" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="154" spans="1:33" ht="24" customHeight="1">
-      <c r="B154" s="8" t="s">
+    <row r="155" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B155" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:33" ht="178" customHeight="1">
-      <c r="B155" s="11"/>
-    </row>
-    <row r="158" spans="1:33" ht="24" customHeight="1">
-      <c r="A158" s="12" t="s">
+    <row r="156" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B156" s="11"/>
+    </row>
+    <row r="159" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="B158" s="12" t="s">
+      <c r="B159" s="12" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="159" spans="1:33" ht="24" customHeight="1">
-      <c r="B159" s="13" t="s">
+    <row r="160" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B160" s="13" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="161" spans="1:33" ht="24" customHeight="1">
-      <c r="A161" s="9" t="s">
+    <row r="162" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="B161" s="9" t="s">
+      <c r="B162" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="162" spans="1:33" ht="24" customHeight="1">
-      <c r="A162" s="14" t="s">
+    <row r="163" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B163" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C162" s="10" t="s">
+      <c r="C163" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="163" spans="1:33" ht="24" customHeight="1">
-      <c r="B163" s="10" t="s">
+    <row r="164" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B164" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:33" ht="24" customHeight="1">
-      <c r="B164" s="11"/>
-      <c r="AA164" s="6" t="s">
+    <row r="165" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B165" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D165" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="AA165" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB164" s="6" t="s">
+      <c r="AB165" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC164" s="6" t="s">
+      <c r="AC165" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD164" s="6" t="s">
+      <c r="AD165" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE164" s="6" t="s">
+      <c r="AE165" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF164" s="6" t="s">
+      <c r="AF165" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG164" s="6" t="s">
+      <c r="AG165" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="166" spans="1:33" ht="24" customHeight="1">
-      <c r="A166" s="9" t="s">
+    <row r="167" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="B166" s="9" t="s">
+      <c r="B167" s="9" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="167" spans="1:33" ht="24" customHeight="1">
-      <c r="A167" s="14" t="s">
+    <row r="168" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B168" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C167" s="10" t="s">
+      <c r="C168" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:33" ht="24" customHeight="1">
-      <c r="B168" s="11"/>
-    </row>
-    <row r="170" spans="1:33" ht="24" customHeight="1">
-      <c r="A170" s="9" t="s">
+    <row r="169" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B169" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="B170" s="9" t="s">
+      <c r="B171" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="171" spans="1:33" ht="24" customHeight="1">
-      <c r="A171" s="14" t="s">
+    <row r="172" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B171" s="10" t="s">
+      <c r="B172" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C171" s="10" t="s">
+      <c r="C172" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="172" spans="1:33" ht="24" customHeight="1">
-      <c r="B172" s="8" t="s">
+    <row r="173" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B173" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="173" spans="1:33" ht="178" customHeight="1">
-      <c r="B173" s="11"/>
-    </row>
-    <row r="176" spans="1:33" ht="24" customHeight="1">
-      <c r="A176" s="12" t="s">
+    <row r="174" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B174" s="11"/>
+    </row>
+    <row r="177" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B176" s="12" t="s">
+      <c r="B177" s="12" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="177" spans="1:33" ht="24" customHeight="1">
-      <c r="B177" s="13" t="s">
+    <row r="178" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B178" s="13" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="179" spans="1:33" ht="24" customHeight="1">
-      <c r="A179" s="9" t="s">
+    <row r="180" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B179" s="9" t="s">
+      <c r="B180" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="180" spans="1:33" ht="24" customHeight="1">
-      <c r="A180" s="14" t="s">
+    <row r="181" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B180" s="10" t="s">
+      <c r="B181" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C180" s="10" t="s">
+      <c r="C181" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="181" spans="1:33" ht="24" customHeight="1">
-      <c r="B181" s="10" t="s">
+    <row r="182" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B182" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:33" ht="24" customHeight="1">
-      <c r="B182" s="11"/>
-      <c r="AA182" s="6" t="s">
+    <row r="183" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B183" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D183" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="AA183" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB182" s="6" t="s">
+      <c r="AB183" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC182" s="6" t="s">
+      <c r="AC183" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD182" s="6" t="s">
+      <c r="AD183" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE182" s="6" t="s">
+      <c r="AE183" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF182" s="6" t="s">
+      <c r="AF183" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG182" s="6" t="s">
+      <c r="AG183" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="184" spans="1:33" ht="24" customHeight="1">
-      <c r="A184" s="9" t="s">
+    <row r="185" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B184" s="9" t="s">
+      <c r="B185" s="9" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="185" spans="1:33" ht="24" customHeight="1">
-      <c r="A185" s="14" t="s">
+    <row r="186" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B186" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C185" s="10" t="s">
+      <c r="C186" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="186" spans="1:33" ht="24" customHeight="1">
-      <c r="B186" s="11"/>
-    </row>
-    <row r="188" spans="1:33" ht="24" customHeight="1">
-      <c r="A188" s="9" t="s">
+    <row r="187" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B187" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B188" s="9" t="s">
+      <c r="B189" s="9" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="189" spans="1:33" ht="24" customHeight="1">
-      <c r="A189" s="14" t="s">
+    <row r="190" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B189" s="10" t="s">
+      <c r="B190" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C189" s="10" t="s">
+      <c r="C190" s="10" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="190" spans="1:33" ht="24" customHeight="1">
-      <c r="B190" s="11"/>
-    </row>
-    <row r="192" spans="1:33" ht="24" customHeight="1">
-      <c r="A192" s="9" t="s">
+    <row r="191" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B191" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B192" s="9" t="s">
+      <c r="B193" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="193" spans="1:33" ht="24" customHeight="1">
-      <c r="A193" s="14" t="s">
+    <row r="194" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B193" s="10" t="s">
+      <c r="B194" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C193" s="10" t="s">
+      <c r="C194" s="10" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="194" spans="1:33" ht="24" customHeight="1">
-      <c r="B194" s="8" t="s">
+    <row r="195" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B195" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="178" customHeight="1">
-      <c r="B195" s="11"/>
-    </row>
-    <row r="198" spans="1:33" ht="24" customHeight="1">
-      <c r="A198" s="12" t="s">
+    <row r="196" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B196" s="11"/>
+    </row>
+    <row r="199" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="B198" s="12" t="s">
+      <c r="B199" s="12" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="199" spans="1:33" ht="24" customHeight="1">
-      <c r="B199" s="13" t="s">
+    <row r="200" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B200" s="13" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:33" ht="24" customHeight="1">
-      <c r="A201" s="9" t="s">
+    <row r="202" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="B201" s="9" t="s">
+      <c r="B202" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="202" spans="1:33" ht="24" customHeight="1">
-      <c r="A202" s="14" t="s">
+    <row r="203" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B202" s="10" t="s">
+      <c r="B203" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C202" s="10" t="s">
+      <c r="C203" s="10" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="203" spans="1:33" ht="24" customHeight="1">
-      <c r="B203" s="10" t="s">
+    <row r="204" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B204" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:33" ht="24" customHeight="1">
-      <c r="B204" s="11"/>
-      <c r="AA204" s="6" t="s">
+    <row r="205" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B205" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D205" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA205" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB204" s="6" t="s">
+      <c r="AB205" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC204" s="6" t="s">
+      <c r="AC205" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD204" s="6" t="s">
+      <c r="AD205" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE204" s="6" t="s">
+      <c r="AE205" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF204" s="6" t="s">
+      <c r="AF205" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG204" s="6" t="s">
+      <c r="AG205" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="206" spans="1:33" ht="24" customHeight="1">
-      <c r="A206" s="9" t="s">
+    <row r="207" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="B206" s="9" t="s">
+      <c r="B207" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="207" spans="1:33" ht="24" customHeight="1">
-      <c r="A207" s="14" t="s">
+    <row r="208" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B207" s="10" t="s">
+      <c r="B208" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C207" s="10" t="s">
+      <c r="C208" s="10" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="208" spans="1:33" ht="24" customHeight="1">
-      <c r="B208" s="8" t="s">
+    <row r="209" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B209" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="209" spans="1:33" ht="178" customHeight="1">
-      <c r="B209" s="11"/>
-    </row>
-    <row r="212" spans="1:33" ht="24" customHeight="1">
-      <c r="A212" s="12" t="s">
+    <row r="210" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B210" s="11"/>
+    </row>
+    <row r="213" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="B212" s="12" t="s">
+      <c r="B213" s="12" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="213" spans="1:33" ht="24" customHeight="1">
-      <c r="B213" s="13" t="s">
+    <row r="214" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B214" s="13" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="215" spans="1:33" ht="24" customHeight="1">
-      <c r="A215" s="9" t="s">
+    <row r="216" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B215" s="9" t="s">
+      <c r="B216" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="216" spans="1:33" ht="24" customHeight="1">
-      <c r="A216" s="14" t="s">
+    <row r="217" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B216" s="10" t="s">
+      <c r="B217" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C216" s="10" t="s">
+      <c r="C217" s="10" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="217" spans="1:33" ht="24" customHeight="1">
-      <c r="B217" s="10" t="s">
+    <row r="218" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B218" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:33" ht="24" customHeight="1">
-      <c r="B218" s="11"/>
-      <c r="AA218" s="6" t="s">
+    <row r="219" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B219" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D219" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="AA219" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB218" s="6" t="s">
+      <c r="AB219" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC218" s="6" t="s">
+      <c r="AC219" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD218" s="6" t="s">
+      <c r="AD219" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE218" s="6" t="s">
+      <c r="AE219" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF218" s="6" t="s">
+      <c r="AF219" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG218" s="6" t="s">
+      <c r="AG219" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="220" spans="1:33" ht="24" customHeight="1">
-      <c r="A220" s="9" t="s">
+    <row r="221" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="B220" s="9" t="s">
+      <c r="B221" s="9" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="221" spans="1:33" ht="24" customHeight="1">
-      <c r="A221" s="14" t="s">
+    <row r="222" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B221" s="10" t="s">
+      <c r="B222" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C221" s="10" t="s">
+      <c r="C222" s="10" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="222" spans="1:33" ht="24" customHeight="1">
-      <c r="B222" s="11"/>
-      <c r="AA222" s="6" t="s">
+    <row r="223" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B223" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D223" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA223" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB222" s="6" t="s">
+      <c r="AB223" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC222" s="6" t="s">
+      <c r="AC223" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD222" s="6" t="s">
+      <c r="AD223" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE222" s="6" t="s">
+      <c r="AE223" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF222" s="6" t="s">
+      <c r="AF223" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="224" spans="1:33" ht="24" customHeight="1">
-      <c r="A224" s="9" t="s">
+    <row r="225" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="B224" s="9" t="s">
+      <c r="B225" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="225" spans="1:33" ht="24" customHeight="1">
-      <c r="A225" s="14" t="s">
+    <row r="226" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B225" s="10" t="s">
+      <c r="B226" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="C225" s="10" t="s">
+      <c r="C226" s="10" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="226" spans="1:33" ht="24" customHeight="1">
-      <c r="B226" s="11"/>
-      <c r="AA226" s="6" t="s">
+    <row r="227" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B227" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D227" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA227" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB226" s="6" t="s">
+      <c r="AB227" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC226" s="6" t="s">
+      <c r="AC227" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD226" s="6" t="s">
+      <c r="AD227" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE226" s="6" t="s">
+      <c r="AE227" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF226" s="6" t="s">
+      <c r="AF227" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="228" spans="1:33" ht="24" customHeight="1">
-      <c r="A228" s="9" t="s">
+    <row r="229" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="B228" s="9" t="s">
+      <c r="B229" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="229" spans="1:33" ht="24" customHeight="1">
-      <c r="A229" s="14" t="s">
+    <row r="230" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B229" s="10" t="s">
+      <c r="B230" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C229" s="10" t="s">
+      <c r="C230" s="10" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="230" spans="1:33" ht="24" customHeight="1">
-      <c r="B230" s="8" t="s">
+    <row r="231" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B231" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="231" spans="1:33" ht="178" customHeight="1">
-      <c r="B231" s="11"/>
-    </row>
-    <row r="234" spans="1:33" ht="24" customHeight="1">
-      <c r="A234" s="12" t="s">
+    <row r="232" spans="1:32" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B232" s="11"/>
+    </row>
+    <row r="235" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B234" s="12" t="s">
+      <c r="B235" s="12" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="235" spans="1:33" ht="24" customHeight="1">
-      <c r="B235" s="13" t="s">
+    <row r="236" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B236" s="13" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="237" spans="1:33" ht="24" customHeight="1">
-      <c r="A237" s="9" t="s">
+    <row r="238" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="B237" s="9" t="s">
+      <c r="B238" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="238" spans="1:33" ht="24" customHeight="1">
-      <c r="A238" s="14" t="s">
+    <row r="239" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B238" s="10" t="s">
+      <c r="B239" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C238" s="10" t="s">
+      <c r="C239" s="10" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="239" spans="1:33" ht="24" customHeight="1">
-      <c r="B239" s="10" t="s">
+    <row r="240" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B240" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:33" ht="24" customHeight="1">
-      <c r="B240" s="11"/>
-      <c r="AA240" s="6" t="s">
+    <row r="241" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B241" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D241" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA241" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB240" s="6" t="s">
+      <c r="AB241" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC240" s="6" t="s">
+      <c r="AC241" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD240" s="6" t="s">
+      <c r="AD241" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE240" s="6" t="s">
+      <c r="AE241" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF240" s="6" t="s">
+      <c r="AF241" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG240" s="6" t="s">
+      <c r="AG241" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="242" spans="1:32" ht="24" customHeight="1">
-      <c r="A242" s="9" t="s">
+    <row r="243" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="B242" s="9" t="s">
+      <c r="B243" s="9" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="243" spans="1:32" ht="24" customHeight="1">
-      <c r="A243" s="14" t="s">
+    <row r="244" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B243" s="10" t="s">
+      <c r="B244" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C243" s="10" t="s">
+      <c r="C244" s="10" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="244" spans="1:32" ht="24" customHeight="1">
-      <c r="B244" s="11"/>
-      <c r="AA244" s="6" t="s">
+    <row r="245" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B245" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D245" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA245" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB244" s="6" t="s">
+      <c r="AB245" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC244" s="6" t="s">
+      <c r="AC245" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD244" s="6" t="s">
+      <c r="AD245" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE244" s="6" t="s">
+      <c r="AE245" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF244" s="6" t="s">
+      <c r="AF245" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="246" spans="1:32" ht="24" customHeight="1">
-      <c r="A246" s="9" t="s">
+    <row r="247" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="B246" s="9" t="s">
+      <c r="B247" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="247" spans="1:32" ht="24" customHeight="1">
-      <c r="A247" s="14" t="s">
+    <row r="248" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B247" s="10" t="s">
+      <c r="B248" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="C247" s="10" t="s">
+      <c r="C248" s="10" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="248" spans="1:32" ht="24" customHeight="1">
-      <c r="B248" s="11"/>
-      <c r="AA248" s="6" t="s">
+    <row r="249" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B249" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D249" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="AA249" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB248" s="6" t="s">
+      <c r="AB249" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC248" s="6" t="s">
+      <c r="AC249" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD248" s="6" t="s">
+      <c r="AD249" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE248" s="6" t="s">
+      <c r="AE249" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF248" s="6" t="s">
+      <c r="AF249" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="250" spans="1:32" ht="24" customHeight="1">
-      <c r="A250" s="9" t="s">
+    <row r="251" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B250" s="9" t="s">
+      <c r="B251" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="251" spans="1:32" ht="24" customHeight="1">
-      <c r="A251" s="14" t="s">
+    <row r="252" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B251" s="10" t="s">
+      <c r="B252" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C251" s="10" t="s">
+      <c r="C252" s="10" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="252" spans="1:32" ht="24" customHeight="1">
-      <c r="B252" s="8" t="s">
+    <row r="253" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B253" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="253" spans="1:32" ht="178" customHeight="1">
-      <c r="B253" s="11"/>
-    </row>
-    <row r="256" spans="1:32" ht="24" customHeight="1">
-      <c r="A256" s="12" t="s">
+    <row r="254" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B254" s="11"/>
+    </row>
+    <row r="257" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="B256" s="12" t="s">
+      <c r="B257" s="12" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="257" spans="1:33" ht="24" customHeight="1">
-      <c r="B257" s="13" t="s">
+    <row r="258" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B258" s="13" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="259" spans="1:33" ht="24" customHeight="1">
-      <c r="A259" s="9" t="s">
+    <row r="260" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B259" s="9" t="s">
+      <c r="B260" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="260" spans="1:33" ht="24" customHeight="1">
-      <c r="A260" s="14" t="s">
+    <row r="261" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B260" s="10" t="s">
+      <c r="B261" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C260" s="10" t="s">
+      <c r="C261" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="261" spans="1:33" ht="24" customHeight="1">
-      <c r="B261" s="10" t="s">
+    <row r="262" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B262" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:33" ht="24" customHeight="1">
-      <c r="B262" s="11"/>
-      <c r="AA262" s="6" t="s">
+    <row r="263" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B263" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D263" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA263" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB262" s="6" t="s">
+      <c r="AB263" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC262" s="6" t="s">
+      <c r="AC263" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD262" s="6" t="s">
+      <c r="AD263" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE262" s="6" t="s">
+      <c r="AE263" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF262" s="6" t="s">
+      <c r="AF263" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG262" s="6" t="s">
+      <c r="AG263" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="264" spans="1:33" ht="24" customHeight="1">
-      <c r="A264" s="9" t="s">
+    <row r="265" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="B264" s="9" t="s">
+      <c r="B265" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="265" spans="1:33" ht="24" customHeight="1">
-      <c r="A265" s="14" t="s">
+    <row r="266" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B265" s="10" t="s">
+      <c r="B266" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C265" s="10" t="s">
+      <c r="C266" s="10" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="266" spans="1:33" ht="24" customHeight="1">
-      <c r="B266" s="8" t="s">
+    <row r="267" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B267" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="267" spans="1:33" ht="178" customHeight="1">
-      <c r="B267" s="11"/>
-    </row>
-    <row r="270" spans="1:33" ht="24" customHeight="1">
-      <c r="A270" s="12" t="s">
+    <row r="268" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B268" s="11"/>
+    </row>
+    <row r="271" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="B270" s="12" t="s">
+      <c r="B271" s="12" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="271" spans="1:33" ht="24" customHeight="1">
-      <c r="B271" s="13" t="s">
+    <row r="272" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B272" s="13" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="273" spans="1:33" ht="24" customHeight="1">
-      <c r="A273" s="9" t="s">
+    <row r="274" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="B273" s="9" t="s">
+      <c r="B274" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="274" spans="1:33" ht="24" customHeight="1">
-      <c r="A274" s="14" t="s">
+    <row r="275" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B274" s="10" t="s">
+      <c r="B275" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C274" s="10" t="s">
+      <c r="C275" s="10" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="275" spans="1:33" ht="24" customHeight="1">
-      <c r="B275" s="10" t="s">
+    <row r="276" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B276" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:33" ht="24" customHeight="1">
-      <c r="B276" s="11"/>
-      <c r="AA276" s="6" t="s">
+    <row r="277" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B277" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D277" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="AA277" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB276" s="6" t="s">
+      <c r="AB277" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC276" s="6" t="s">
+      <c r="AC277" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD276" s="6" t="s">
+      <c r="AD277" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE276" s="6" t="s">
+      <c r="AE277" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF276" s="6" t="s">
+      <c r="AF277" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG276" s="6" t="s">
+      <c r="AG277" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="278" spans="1:33" ht="24" customHeight="1">
-      <c r="A278" s="9" t="s">
+    <row r="279" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B278" s="9" t="s">
+      <c r="B279" s="9" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="279" spans="1:33" ht="24" customHeight="1">
-      <c r="A279" s="14" t="s">
+    <row r="280" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B279" s="10" t="s">
+      <c r="B280" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C279" s="10" t="s">
+      <c r="C280" s="10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="280" spans="1:33" ht="24" customHeight="1">
-      <c r="B280" s="11"/>
-    </row>
-    <row r="282" spans="1:33" ht="24" customHeight="1">
-      <c r="A282" s="9" t="s">
+    <row r="281" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B281" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="B282" s="9" t="s">
+      <c r="B283" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="283" spans="1:33" ht="24" customHeight="1">
-      <c r="A283" s="14" t="s">
+    <row r="284" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B283" s="10" t="s">
+      <c r="B284" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C283" s="10" t="s">
+      <c r="C284" s="10" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="284" spans="1:33" ht="24" customHeight="1">
-      <c r="B284" s="8" t="s">
+    <row r="285" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B285" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="285" spans="1:33" ht="178" customHeight="1">
-      <c r="B285" s="11"/>
-    </row>
-    <row r="288" spans="1:33" ht="24" customHeight="1">
-      <c r="A288" s="12" t="s">
+    <row r="286" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B286" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="289" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B288" s="12" t="s">
+      <c r="B289" s="12" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="289" spans="1:32" ht="24" customHeight="1">
-      <c r="B289" s="13" t="s">
+    <row r="290" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B290" s="13" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="291" spans="1:32" ht="24" customHeight="1">
-      <c r="A291" s="9" t="s">
+    <row r="292" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A292" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="B291" s="9" t="s">
+      <c r="B292" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="292" spans="1:32" ht="24" customHeight="1">
-      <c r="A292" s="14" t="s">
+    <row r="293" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A293" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B292" s="10" t="s">
+      <c r="B293" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C292" s="10" t="s">
+      <c r="C293" s="10" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="293" spans="1:32" ht="24" customHeight="1">
-      <c r="B293" s="10" t="s">
+    <row r="294" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B294" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="294" spans="1:32" ht="24" customHeight="1">
-      <c r="B294" s="11"/>
-      <c r="AA294" s="6" t="s">
+    <row r="295" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B295" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="AA295" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="AB294" s="6" t="s">
+      <c r="AB295" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="AC294" s="6" t="s">
+      <c r="AC295" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="AD294" s="6" t="s">
+      <c r="AD295" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="AE294" s="6" t="s">
+      <c r="AE295" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="AF294" s="6" t="s">
+      <c r="AF295" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="296" spans="1:32" ht="24" customHeight="1">
-      <c r="A296" s="9" t="s">
+    <row r="297" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="B296" s="9" t="s">
+      <c r="B297" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="297" spans="1:32" ht="24" customHeight="1">
-      <c r="A297" s="14" t="s">
+    <row r="298" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B297" s="10" t="s">
+      <c r="B298" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C297" s="10" t="s">
+      <c r="C298" s="10" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="298" spans="1:32" ht="24" customHeight="1">
-      <c r="B298" s="8" t="s">
+    <row r="299" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B299" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="299" spans="1:32" ht="178" customHeight="1">
-      <c r="B299" s="11"/>
+    <row r="300" spans="1:32" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B300" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="27">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B277 B263 B241 B219 B205 B183 B165 B151 B137 B123 B109 B91 B77 B63 B49 B20:B21" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>AA20:AG20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
-      <formula1>AA34:AG34</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B95" xr:uid="{00000000-0002-0000-0300-000006000000}">
+      <formula1>AA95:AE95</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
-      <formula1>AA48:AG48</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
-      <formula1>AA62:AG62</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>AA76:AG76</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90">
-      <formula1>AA90:AG90</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B94">
-      <formula1>AA94:AE94</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B108">
-      <formula1>AA108:AG108</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122">
-      <formula1>AA122:AG122</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B136">
-      <formula1>AA136:AG136</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B150">
-      <formula1>AA150:AG150</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B164">
-      <formula1>AA164:AG164</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B168">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B169 B281 B191 B187" xr:uid="{00000000-0002-0000-0300-00000C000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B182">
-      <formula1>AA182:AG182</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B186">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B190">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B204">
-      <formula1>AA204:AG204</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B218">
-      <formula1>AA218:AG218</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B222">
-      <formula1>AA222:AF222</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B226">
-      <formula1>AA226:AF226</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B240">
-      <formula1>AA240:AG240</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B244">
-      <formula1>AA244:AF244</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B248">
-      <formula1>AA248:AF248</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B262">
-      <formula1>AA262:AG262</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B276">
-      <formula1>AA276:AG276</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B280">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B294">
-      <formula1>AA294:AF294</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B223 B295 B249 B245 B227" xr:uid="{00000000-0002-0000-0300-000012000000}">
+      <formula1>AA223:AF223</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix some cmcc-esm2 toplevel attributes
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
+++ b/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-esm2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0891E754-4EA7-C341-9786-31A7A14A6287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC450C29-8624-4E43-8BE0-FE5F8CA2A8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -1321,9 +1321,6 @@
     <t>Land Use Harmonization version 2 (LUH2) is used after conversion to CLM plant functional and landunit types.</t>
   </si>
   <si>
-    <t>CMCC, CESM, climate model</t>
-  </si>
-  <si>
     <t>No fluxes corrections are used in the model.</t>
   </si>
   <si>
@@ -1406,6 +1403,9 @@
   </si>
   <si>
     <t>CMCC-ESM2</t>
+  </si>
+  <si>
+    <t>CMCC, CESM, Earth System Model</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2040,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -2110,18 +2110,18 @@
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>456</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2248,7 +2248,7 @@
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>432</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2317,7 +2317,7 @@
     </row>
     <row r="25" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2429,7 +2429,7 @@
     </row>
     <row r="46" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2561,7 +2561,7 @@
     </row>
     <row r="71" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2588,7 +2588,7 @@
         <v>111</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AA75" s="6" t="s">
         <v>104</v>
@@ -2749,7 +2749,7 @@
     </row>
     <row r="100" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2860,7 +2860,7 @@
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2884,7 +2884,7 @@
     </row>
     <row r="123" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2926,7 +2926,7 @@
     </row>
     <row r="132" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2955,7 +2955,7 @@
     </row>
     <row r="137" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2984,7 +2984,7 @@
     </row>
     <row r="142" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3013,7 +3013,7 @@
     </row>
     <row r="147" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3042,7 +3042,7 @@
     </row>
     <row r="152" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3071,7 +3071,7 @@
     </row>
     <row r="157" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3113,7 +3113,7 @@
     </row>
     <row r="166" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,7 +3142,7 @@
     </row>
     <row r="171" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3171,7 +3171,7 @@
     </row>
     <row r="176" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3200,7 +3200,7 @@
     </row>
     <row r="181" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3229,7 +3229,7 @@
     </row>
     <row r="186" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,7 +3258,7 @@
     </row>
     <row r="191" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3314,7 +3314,7 @@
     </row>
     <row r="201" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3383,7 +3383,7 @@
     </row>
     <row r="215" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3427,7 +3427,7 @@
       <c r="B224" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA75:AH75</formula1>
     </dataValidation>
@@ -3446,7 +3446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AG300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update description of changes for cmcc-esm2
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
+++ b/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-esm2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/es-doc.cmcc/cmip6/models/cmcc-esm2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC450C29-8624-4E43-8BE0-FE5F8CA2A8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA305393-04F5-9644-8206-D94C7C45A3C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1336,9 +1336,6 @@
     <t>CPL6/MCT</t>
   </si>
   <si>
-    <t>In comparison to its previous version, the model contains many substantial science and infrastructure changes and improvements in all its components. These new advancements include: a different atmospheric model component (CAM) that incorporates significantly advanced features for turbulence and convection representations; a different land model component (CLM) with increase number of PFT components and updated land processes representation; a community based seaice model (CICE) with state of the art thermodyanics formulations and additioanl parameerizations; an updated ocean component (NEMO) with additional features to describe ocean interior dynamics, small scale paramterizations and improved computational capabilities.</t>
-  </si>
-  <si>
     <t>The details of the model tuning will be described in the CMCC model description manuscript. The primary tuning involved the top-of-the-atmosphere (TOA) heat flux in pre-industrial control simulations. Our desire was to achive a rather small TOA (e.g. &lt; 0.1 W m^-2), mostly working on atmospheric aerosol indiret effects and land processes related to the snow cycle in northern emisphere.</t>
   </si>
   <si>
@@ -1406,6 +1403,9 @@
   </si>
   <si>
     <t>CMCC, CESM, Earth System Model</t>
+  </si>
+  <si>
+    <t>In comparison to its previous version, the model contains many substantial science and infrastructure changes and improvements in all its components. These new advancements include: a different atmospheric model component (CAM) that incorporates significantly advanced features for turbulence and convection representations; a different land model component (CLM) with increase number of PFT components and updated land processes representation; a community based seaice model (CICE) with state of the art thermodyanics formulations and additioanl parameerizations; an updated ocean component (NEMO) with additional features to describe ocean interior dynamics, small scale paramterizations and improved computational capabilities. Marine biogeochemistry (BFM) is resolved for an intermediate complexity ecosystem structure, with the explicit heterotrophic bacteria, and includes an interactive benthic compartment.</t>
   </si>
 </sst>
 </file>
@@ -2040,7 +2040,7 @@
         <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -2110,18 +2110,18 @@
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>455</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2248,7 +2248,7 @@
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2429,7 +2429,7 @@
     </row>
     <row r="46" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2749,7 +2749,7 @@
     </row>
     <row r="100" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2807,7 +2807,7 @@
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2860,7 +2860,7 @@
     </row>
     <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2884,7 +2884,7 @@
     </row>
     <row r="123" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2926,7 +2926,7 @@
     </row>
     <row r="132" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2955,7 +2955,7 @@
     </row>
     <row r="137" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2984,7 +2984,7 @@
     </row>
     <row r="142" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3013,7 +3013,7 @@
     </row>
     <row r="147" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3042,7 +3042,7 @@
     </row>
     <row r="152" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3071,7 +3071,7 @@
     </row>
     <row r="157" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3113,7 +3113,7 @@
     </row>
     <row r="166" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,7 +3142,7 @@
     </row>
     <row r="171" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3171,7 +3171,7 @@
     </row>
     <row r="176" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3200,7 +3200,7 @@
     </row>
     <row r="181" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3229,7 +3229,7 @@
     </row>
     <row r="186" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,7 +3258,7 @@
     </row>
     <row r="191" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3314,7 +3314,7 @@
     </row>
     <row r="201" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3383,7 +3383,7 @@
     </row>
     <row r="215" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add info for cmcc-esm2
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
+++ b/cmip6/models/cmcc-esm2/cmip6_cmcc_cmcc-esm2_toplevel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/es-doc.cmcc/cmip6/models/cmcc-esm2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA305393-04F5-9644-8206-D94C7C45A3C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989A321-AF07-5544-B40B-C17016D4BF35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1402,10 +1402,10 @@
     <t>CMCC-ESM2</t>
   </si>
   <si>
-    <t>CMCC, CESM, Earth System Model</t>
-  </si>
-  <si>
     <t>In comparison to its previous version, the model contains many substantial science and infrastructure changes and improvements in all its components. These new advancements include: a different atmospheric model component (CAM) that incorporates significantly advanced features for turbulence and convection representations; a different land model component (CLM) with increase number of PFT components and updated land processes representation; a community based seaice model (CICE) with state of the art thermodyanics formulations and additioanl parameerizations; an updated ocean component (NEMO) with additional features to describe ocean interior dynamics, small scale paramterizations and improved computational capabilities. Marine biogeochemistry (BFM) is resolved for an intermediate complexity ecosystem structure, with the explicit heterotrophic bacteria, and includes an interactive benthic compartment.</t>
+  </si>
+  <si>
+    <t>CMCC, Earth System Model, coupled-climate-carbon cycles</t>
   </si>
 </sst>
 </file>
@@ -2173,8 +2173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -2429,7 +2429,7 @@
     </row>
     <row r="46" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>